<commit_message>
se consigue leer la matriz de contutividades K que viene de la tabla excel
</commit_message>
<xml_diff>
--- a/teidecode_v1/Thermal_Data.xlsx
+++ b/teidecode_v1/Thermal_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erjav\Desktop\TeideThermal\TeideThermal\teidecode_v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tesar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4363B46-62C3-4EA1-B198-0FA1E67BDDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CA31B0-EB46-4605-A42D-5D7D6FD194E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes properties" sheetId="1" r:id="rId1"/>
@@ -2022,19 +2022,19 @@
       <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="26.453125" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" customWidth="1"/>
+    <col min="13" max="13" width="10.81640625" customWidth="1"/>
+    <col min="14" max="14" width="8.1796875" customWidth="1"/>
+    <col min="15" max="15" width="8.54296875" customWidth="1"/>
     <col min="16" max="16" width="31" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" customWidth="1"/>
+    <col min="18" max="18" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -7937,20 +7937,20 @@
   <dimension ref="A1:AD990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="O21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="AC34" sqref="AC34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
     <col min="2" max="10" width="7" customWidth="1"/>
-    <col min="11" max="30" width="8.140625" customWidth="1"/>
+    <col min="11" max="30" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" ht="14.5">
       <c r="A1" s="20" t="s">
         <v>143</v>
       </c>
@@ -7984,7 +7984,7 @@
       <c r="AC1" s="21"/>
       <c r="AD1" s="21"/>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" ht="14.5">
       <c r="A2" s="20" t="s">
         <v>144</v>
       </c>
@@ -8018,7 +8018,7 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="21"/>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" ht="14.5">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -8050,7 +8050,7 @@
       <c r="AC3" s="21"/>
       <c r="AD3" s="21"/>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" ht="14.5">
       <c r="A4" s="22" t="s">
         <v>145</v>
       </c>
@@ -8142,7 +8142,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" ht="14.5">
       <c r="A5" s="22" t="s">
         <v>25</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" ht="14.5">
       <c r="A6" s="22" t="s">
         <v>32</v>
       </c>
@@ -8341,7 +8341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" ht="14.5">
       <c r="A7" s="22" t="s">
         <v>36</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" ht="14.5">
       <c r="A8" s="22" t="s">
         <v>41</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" ht="14.5">
       <c r="A9" s="22" t="s">
         <v>46</v>
       </c>
@@ -8635,7 +8635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" ht="14.5">
       <c r="A10" s="22" t="s">
         <v>51</v>
       </c>
@@ -8735,7 +8735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" ht="14.5">
       <c r="A11" s="22" t="s">
         <v>56</v>
       </c>
@@ -8838,7 +8838,7 @@
         <v>0.26367831245880025</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" ht="14.5">
       <c r="A12" s="22" t="s">
         <v>61</v>
       </c>
@@ -8937,7 +8937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" ht="14.5">
       <c r="A13" s="22" t="s">
         <v>67</v>
       </c>
@@ -9037,7 +9037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" ht="14.5">
       <c r="A14" s="22" t="s">
         <v>69</v>
       </c>
@@ -11250,7 +11250,9 @@
         <f>AD31</f>
         <v>0</v>
       </c>
-      <c r="AC33" s="27"/>
+      <c r="AC33" s="27">
+        <v>0</v>
+      </c>
       <c r="AD33" s="24">
         <v>0</v>
       </c>
@@ -41898,11 +41900,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.26953125" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
se deja comentado lo que sobresribe el strcut de datos, ahora funciona pero no esta leyendo el excel
</commit_message>
<xml_diff>
--- a/teidecode_v1/Thermal_Data.xlsx
+++ b/teidecode_v1/Thermal_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tesar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erjav\Desktop\TeideThermal\TeideThermal\teidecode_v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CA31B0-EB46-4605-A42D-5D7D6FD194E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD164C9-77A6-4CFC-992C-5C08B12207BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes properties" sheetId="1" r:id="rId1"/>
@@ -216,6 +216,165 @@
         </r>
       </text>
     </comment>
+    <comment ref="D40" authorId="0" shapeId="0" xr:uid="{42EEAE3D-C9E1-4214-929A-32E846AA4EE3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Thermal capacitance
+======</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E40" authorId="0" shapeId="0" xr:uid="{7311E67F-6B54-428D-9549-C49AA7473EA0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Superficie que queda expuesta a la luz solar.
+======
+ID#AAAAZdRQ90w
+Laura Feria del Rosario    (2022-05-22 21:04:23)
+Recalcular</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{D569FC78-257C-4A40-9FA5-D0BC220C126F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Vector normal a la superficie (para la incidencia solar)
+======
+ID#AAAAaj4eTTo
+Laura Feria del Rosario    (2022-06-04 14:02:02)
+sólo para los que den al exterior?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G40" authorId="0" shapeId="0" xr:uid="{63CD2D35-E740-4BC5-AD94-0011FDC1958E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Emisividad en infrarrojo
+======
+ID#AAAAaj4eTTg
+Laura Feria del Rosario    (2022-06-04 14:00:33)
+sólo para los que den al exterior?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H40" authorId="0" shapeId="0" xr:uid="{54068593-D059-4EF2-94ED-E167393A18BF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>absortividad (en solar)
+======
+ID#AAAAaj4eTTk
+Laura Feria del Rosario    (2022-06-04 14:00:38)
+sólo para los que den al exterior?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I40" authorId="0" shapeId="0" xr:uid="{0A3720CD-F152-4FFB-B14B-9BAC8D342C07}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>nodos con los que esta conectado el nodo en cuestión. El nodo 0 es el espacio exterior
+======</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J40" authorId="0" shapeId="0" xr:uid="{ACE908E4-D0E6-4F6E-A766-07EECCD44709}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Calor generado
+======</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K40" authorId="0" shapeId="0" xr:uid="{5316AA06-C0CB-419C-943B-78A2DE5EDAFA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Thermal conductivity
+======</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L40" authorId="0" shapeId="0" xr:uid="{3BCC13AD-C8CA-4005-9AA7-FCDD0022CC70}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Distancia entre los centros de cada nodo (distancia recorrida por el flujo del calor)
+======
+ID#AAAAaj4eTTY
+Laura Feria del Rosario    (2022-06-04 13:55:37)
+no entiendo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J69" authorId="0" shapeId="0" xr:uid="{4DF5F109-BBD4-4683-8B2A-3BFB0D97FD28}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAZgExsII
+Javier González Vilar    (2022-05-23 14:27:20)
+@teidesat29@ull.edu.es
+cual es la generación de calor del eps de alta?
+_Asignado a Juan Francisco Hernández Cabrera_</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
   <extLst>
     <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion1">
@@ -271,7 +430,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="213">
   <si>
     <t>Esta tabla representado el struct con todos los datos de entrada que uso para el satélite,¿que le falta? pues el coeficiente Cp (specific heat capacity ) esta bastamente aproximado y habría que mirar material por material, puede que algo de info útil pueda ser encontrada en la tabla de mecánica</t>
   </si>
@@ -1382,7 +1541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1522,6 +1681,15 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1641,10 +1809,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>-1724025</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6753225" cy="5038725"/>
     <xdr:pic>
@@ -1665,6 +1833,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7353300" y="6448425"/>
+          <a:ext cx="6753225" cy="5038725"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1675,10 +1847,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6981825" cy="4943475"/>
     <xdr:pic>
@@ -1699,6 +1871,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14106525" y="6353175"/>
+          <a:ext cx="6981825" cy="4943475"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -2015,26 +2191,26 @@
   </sheetPr>
   <dimension ref="A1:AD995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6:Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="31.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" customWidth="1"/>
-    <col min="5" max="5" width="26.453125" customWidth="1"/>
-    <col min="10" max="10" width="16.54296875" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" customWidth="1"/>
-    <col min="13" max="13" width="10.81640625" customWidth="1"/>
-    <col min="14" max="14" width="8.1796875" customWidth="1"/>
-    <col min="15" max="15" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" customWidth="1"/>
     <col min="16" max="16" width="31" customWidth="1"/>
-    <col min="18" max="18" width="18.453125" customWidth="1"/>
+    <col min="18" max="18" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -3997,269 +4173,1222 @@
       <c r="P38" s="19"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="19"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
     </row>
     <row r="40" spans="1:17">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
+      <c r="A40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41" spans="1:17">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="19"/>
-      <c r="L41" s="19"/>
+      <c r="A41" s="75" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="71">
+        <v>4.0648000000000004E-2</v>
+      </c>
+      <c r="D41" s="78">
+        <v>896</v>
+      </c>
+      <c r="E41" s="71">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="F41" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="H41" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="I41" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="J41" s="71">
+        <v>0</v>
+      </c>
+      <c r="K41" s="71">
+        <v>167</v>
+      </c>
+      <c r="L41" s="71" t="s">
+        <v>29</v>
+      </c>
       <c r="M41" s="19"/>
       <c r="N41" s="19"/>
       <c r="O41" s="19"/>
       <c r="P41" s="19"/>
     </row>
     <row r="42" spans="1:17">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="19"/>
-      <c r="L42" s="19"/>
+      <c r="A42" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="72">
+        <v>4.0648000000000004E-2</v>
+      </c>
+      <c r="D42" s="78">
+        <v>896</v>
+      </c>
+      <c r="E42" s="72">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="F42" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="H42" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="I42" s="72" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="72">
+        <v>0</v>
+      </c>
+      <c r="K42" s="72">
+        <v>167</v>
+      </c>
+      <c r="L42" s="72" t="s">
+        <v>29</v>
+      </c>
       <c r="M42" s="19"/>
       <c r="N42" s="19"/>
       <c r="O42" s="19"/>
       <c r="P42" s="19"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="19"/>
-      <c r="L43" s="19"/>
+      <c r="A43" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="71">
+        <v>7.2910000000000006E-3</v>
+      </c>
+      <c r="D43" s="78">
+        <v>896</v>
+      </c>
+      <c r="E43" s="71">
+        <v>0</v>
+      </c>
+      <c r="F43" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="G43" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="H43" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="I43" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="J43" s="71">
+        <v>0</v>
+      </c>
+      <c r="K43" s="71">
+        <v>167</v>
+      </c>
+      <c r="L43" s="71" t="s">
+        <v>29</v>
+      </c>
       <c r="M43" s="19"/>
       <c r="N43" s="19"/>
       <c r="O43" s="19"/>
       <c r="P43" s="19"/>
     </row>
     <row r="44" spans="1:17">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="19"/>
-      <c r="L44" s="19"/>
+      <c r="A44" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="72">
+        <v>7.3419999999999996E-3</v>
+      </c>
+      <c r="D44" s="78">
+        <v>896</v>
+      </c>
+      <c r="E44" s="72">
+        <v>0</v>
+      </c>
+      <c r="F44" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="G44" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="H44" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="I44" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="J44" s="72">
+        <v>0</v>
+      </c>
+      <c r="K44" s="72">
+        <v>167</v>
+      </c>
+      <c r="L44" s="72" t="s">
+        <v>29</v>
+      </c>
       <c r="M44" s="19"/>
       <c r="N44" s="19"/>
       <c r="O44" s="19"/>
       <c r="P44" s="19"/>
     </row>
     <row r="45" spans="1:17">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="19"/>
-      <c r="L45" s="19"/>
+      <c r="A45" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="71">
+        <v>6.4250000000000002E-3</v>
+      </c>
+      <c r="D45" s="78">
+        <v>896</v>
+      </c>
+      <c r="E45" s="71">
+        <v>0</v>
+      </c>
+      <c r="F45" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="H45" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="I45" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="J45" s="71">
+        <v>0</v>
+      </c>
+      <c r="K45" s="71">
+        <v>167</v>
+      </c>
+      <c r="L45" s="71" t="s">
+        <v>29</v>
+      </c>
       <c r="M45" s="19"/>
       <c r="N45" s="19"/>
       <c r="O45" s="19"/>
       <c r="P45" s="19"/>
     </row>
     <row r="46" spans="1:17">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="19"/>
-      <c r="L46" s="19"/>
+      <c r="A46" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="72">
+        <v>6.2350000000000001E-3</v>
+      </c>
+      <c r="D46" s="78">
+        <v>896</v>
+      </c>
+      <c r="E46" s="72">
+        <v>0</v>
+      </c>
+      <c r="F46" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="G46" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="H46" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="I46" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="J46" s="72">
+        <v>0</v>
+      </c>
+      <c r="K46" s="72">
+        <v>167</v>
+      </c>
+      <c r="L46" s="72" t="s">
+        <v>29</v>
+      </c>
       <c r="M46" s="19"/>
       <c r="N46" s="19"/>
       <c r="O46" s="19"/>
       <c r="P46" s="19"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="19"/>
-      <c r="L47" s="19"/>
+      <c r="A47" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="71">
+        <v>2.1920000000000002E-2</v>
+      </c>
+      <c r="D47" s="78">
+        <v>896</v>
+      </c>
+      <c r="E47" s="71">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="F47" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="G47" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="H47" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="I47" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="J47" s="71">
+        <v>0</v>
+      </c>
+      <c r="K47" s="71">
+        <v>167</v>
+      </c>
+      <c r="L47" s="71" t="s">
+        <v>29</v>
+      </c>
       <c r="M47" s="19"/>
       <c r="N47" s="19"/>
       <c r="O47" s="19"/>
       <c r="P47" s="19"/>
     </row>
     <row r="48" spans="1:17">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="19"/>
-      <c r="L48" s="19"/>
+      <c r="A48" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="72">
+        <v>1.8E-3</v>
+      </c>
+      <c r="D48" s="78">
+        <v>1000</v>
+      </c>
+      <c r="E48" s="72">
+        <v>5.7600000000000001E-4</v>
+      </c>
+      <c r="F48" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="G48" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="H48" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="I48" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="J48" s="72">
+        <v>0</v>
+      </c>
+      <c r="K48" s="72">
+        <v>0.188</v>
+      </c>
+      <c r="L48" s="72" t="s">
+        <v>29</v>
+      </c>
       <c r="M48" s="19"/>
       <c r="N48" s="19"/>
       <c r="O48" s="19"/>
       <c r="P48" s="19"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="19"/>
-      <c r="L49" s="19"/>
+      <c r="A49" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="71">
+        <v>1.8E-3</v>
+      </c>
+      <c r="D49" s="78">
+        <v>1000</v>
+      </c>
+      <c r="E49" s="71">
+        <v>5.7600000000000001E-4</v>
+      </c>
+      <c r="F49" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="G49" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="H49" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="I49" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="J49" s="71">
+        <v>0</v>
+      </c>
+      <c r="K49" s="71">
+        <v>0.188</v>
+      </c>
+      <c r="L49" s="71" t="s">
+        <v>29</v>
+      </c>
       <c r="M49" s="19"/>
       <c r="N49" s="19"/>
       <c r="O49" s="19"/>
       <c r="P49" s="19"/>
     </row>
     <row r="50" spans="1:16">
-      <c r="C50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="A50" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="72">
+        <v>1.8E-3</v>
+      </c>
+      <c r="D50" s="78">
+        <v>1000</v>
+      </c>
+      <c r="E50" s="72">
+        <v>5.7600000000000001E-4</v>
+      </c>
+      <c r="F50" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="G50" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="H50" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="I50" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="J50" s="72">
+        <v>0</v>
+      </c>
+      <c r="K50" s="72">
+        <v>0.188</v>
+      </c>
+      <c r="L50" s="72" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="51" spans="1:16">
-      <c r="C51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="A51" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="71">
+        <v>1.8E-3</v>
+      </c>
+      <c r="D51" s="78">
+        <v>1000</v>
+      </c>
+      <c r="E51" s="71">
+        <v>5.7600000000000001E-4</v>
+      </c>
+      <c r="F51" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="G51" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="H51" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="I51" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="J51" s="71">
+        <v>0</v>
+      </c>
+      <c r="K51" s="71">
+        <v>0.188</v>
+      </c>
+      <c r="L51" s="71" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="52" spans="1:16">
-      <c r="C52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="A52" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="72">
+        <v>2.375E-2</v>
+      </c>
+      <c r="D52" s="78">
+        <v>1100</v>
+      </c>
+      <c r="E52" s="72">
+        <v>0</v>
+      </c>
+      <c r="F52" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="G52" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="H52" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="I52" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="J52" s="72">
+        <v>0</v>
+      </c>
+      <c r="K52" s="72">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L52" s="72" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="53" spans="1:16">
-      <c r="C53" s="1"/>
-      <c r="E53" s="1"/>
+      <c r="A53" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="71">
+        <v>0.12590999999999999</v>
+      </c>
+      <c r="D53" s="78">
+        <v>800</v>
+      </c>
+      <c r="E53" s="71">
+        <v>0</v>
+      </c>
+      <c r="F53" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="G53" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="H53" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="I53" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="J53" s="71">
+        <v>0</v>
+      </c>
+      <c r="K53" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L53" s="71" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="54" spans="1:16">
-      <c r="C54" s="1"/>
-      <c r="E54" s="1"/>
+      <c r="A54" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="72">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D54" s="78">
+        <v>932.5</v>
+      </c>
+      <c r="E54" s="72">
+        <v>0</v>
+      </c>
+      <c r="F54" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="G54" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="I54" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="J54" s="72">
+        <v>0.5</v>
+      </c>
+      <c r="K54" s="72">
+        <v>0.4</v>
+      </c>
+      <c r="L54" s="72" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="55" spans="1:16">
-      <c r="C55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="A55" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="71">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D55" s="78">
+        <v>932.5</v>
+      </c>
+      <c r="E55" s="71">
+        <v>0</v>
+      </c>
+      <c r="F55" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="H55" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="I55" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="J55" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="K55" s="71">
+        <v>0.4</v>
+      </c>
+      <c r="L55" s="71" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="56" spans="1:16">
-      <c r="C56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="A56" s="76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="72">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D56" s="78">
+        <v>932.5</v>
+      </c>
+      <c r="E56" s="72">
+        <v>0</v>
+      </c>
+      <c r="F56" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="H56" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="I56" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="J56" s="72">
+        <v>0.5</v>
+      </c>
+      <c r="K56" s="72">
+        <v>0.4</v>
+      </c>
+      <c r="L56" s="72" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="57" spans="1:16">
-      <c r="C57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="A57" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="71">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D57" s="78">
+        <v>932.5</v>
+      </c>
+      <c r="E57" s="71">
+        <v>0</v>
+      </c>
+      <c r="F57" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="H57" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="I57" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="J57" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="K57" s="71">
+        <v>0.4</v>
+      </c>
+      <c r="L57" s="71" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="58" spans="1:16">
-      <c r="C58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="A58" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="72">
+        <v>0.05</v>
+      </c>
+      <c r="D58" s="78">
+        <v>1000</v>
+      </c>
+      <c r="E58" s="72">
+        <v>0</v>
+      </c>
+      <c r="F58" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="H58" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="I58" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="J58" s="72">
+        <v>0.1</v>
+      </c>
+      <c r="K58" s="72">
+        <v>1.17</v>
+      </c>
+      <c r="L58" s="72" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="59" spans="1:16">
-      <c r="C59" s="1"/>
-      <c r="E59" s="1"/>
+      <c r="A59" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="71">
+        <v>0.05</v>
+      </c>
+      <c r="D59" s="78">
+        <v>1000</v>
+      </c>
+      <c r="E59" s="71">
+        <v>0</v>
+      </c>
+      <c r="F59" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="H59" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="I59" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="J59" s="71">
+        <v>0</v>
+      </c>
+      <c r="K59" s="71">
+        <v>1.17</v>
+      </c>
+      <c r="L59" s="71" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="60" spans="1:16">
-      <c r="C60" s="1"/>
-      <c r="E60" s="1"/>
+      <c r="A60" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="C60" s="72">
+        <v>3.8490000000000003E-2</v>
+      </c>
+      <c r="D60" s="78">
+        <v>1100</v>
+      </c>
+      <c r="E60" s="72">
+        <v>0</v>
+      </c>
+      <c r="F60" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="G60" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="H60" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="I60" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="J60" s="72">
+        <v>0.5</v>
+      </c>
+      <c r="K60" s="72">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L60" s="72" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="61" spans="1:16">
-      <c r="C61" s="1"/>
-      <c r="E61" s="1"/>
+      <c r="A61" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="B61" s="71" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="71">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D61" s="78">
+        <v>1100</v>
+      </c>
+      <c r="E61" s="71">
+        <v>0</v>
+      </c>
+      <c r="F61" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="H61" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="I61" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="J61" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="K61" s="71">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L61" s="71" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="C62" s="1"/>
-      <c r="E62" s="1"/>
+      <c r="A62" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="72" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" s="72">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D62" s="78">
+        <v>857.4</v>
+      </c>
+      <c r="E62" s="72">
+        <v>0</v>
+      </c>
+      <c r="F62" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="G62" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="H62" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="I62" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="J62" s="72">
+        <v>2</v>
+      </c>
+      <c r="K62" s="72">
+        <v>167</v>
+      </c>
+      <c r="L62" s="72">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="63" spans="1:16">
-      <c r="C63" s="1"/>
-      <c r="E63" s="1"/>
+      <c r="A63" s="75" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" s="71">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D63" s="78">
+        <v>1100</v>
+      </c>
+      <c r="E63" s="71">
+        <v>0</v>
+      </c>
+      <c r="F63" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="G63" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="H63" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="I63" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="J63" s="77">
+        <v>1.5</v>
+      </c>
+      <c r="K63" s="71">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L63" s="71" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="64" spans="1:16">
-      <c r="C64" s="1"/>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="3:5">
-      <c r="C65" s="1"/>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="3:5">
-      <c r="C66" s="1"/>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="3:5">
-      <c r="C67" s="1"/>
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="3:5">
-      <c r="C68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="3:5">
-      <c r="C69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="3:5">
+      <c r="A64" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" s="72" t="s">
+        <v>117</v>
+      </c>
+      <c r="C64" s="72">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D64" s="78">
+        <v>703</v>
+      </c>
+      <c r="E64" s="72">
+        <v>8.0940000000000005E-3</v>
+      </c>
+      <c r="F64" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="G64" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="H64" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="I64" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J64" s="72">
+        <v>2.4</v>
+      </c>
+      <c r="K64" s="72">
+        <v>0.35</v>
+      </c>
+      <c r="L64" s="72">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" s="71" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="71">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D65" s="78">
+        <v>703</v>
+      </c>
+      <c r="E65" s="71">
+        <v>8.0940000000000005E-3</v>
+      </c>
+      <c r="F65" s="71" t="s">
+        <v>125</v>
+      </c>
+      <c r="G65" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="H65" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="I65" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="J65" s="71">
+        <v>2.4</v>
+      </c>
+      <c r="K65" s="71">
+        <v>0.35</v>
+      </c>
+      <c r="L65" s="71">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="76" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="72">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D66" s="78">
+        <v>703</v>
+      </c>
+      <c r="E66" s="72">
+        <v>8.0940000000000005E-3</v>
+      </c>
+      <c r="F66" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="H66" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="I66" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="J66" s="72">
+        <v>2.4</v>
+      </c>
+      <c r="K66" s="72">
+        <v>0.35</v>
+      </c>
+      <c r="L66" s="72">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="71">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D67" s="78">
+        <v>703</v>
+      </c>
+      <c r="E67" s="71">
+        <v>8.0940000000000005E-3</v>
+      </c>
+      <c r="F67" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="H67" s="71">
+        <v>0.8</v>
+      </c>
+      <c r="I67" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="J67" s="71">
+        <v>2.4</v>
+      </c>
+      <c r="K67" s="71">
+        <v>0.35</v>
+      </c>
+      <c r="L67" s="71">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="76" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="72" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="72">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="D68" s="78">
+        <v>703</v>
+      </c>
+      <c r="E68" s="72">
+        <v>8.4469999999999996E-3</v>
+      </c>
+      <c r="F68" s="72" t="s">
+        <v>137</v>
+      </c>
+      <c r="G68" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="H68" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="I68" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="J68" s="72">
+        <v>2.4</v>
+      </c>
+      <c r="K68" s="72">
+        <v>0.35</v>
+      </c>
+      <c r="L68" s="72">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="75" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" s="71">
+        <v>0.04</v>
+      </c>
+      <c r="D69" s="79">
+        <v>1100</v>
+      </c>
+      <c r="E69" s="71">
+        <v>0</v>
+      </c>
+      <c r="F69" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="G69" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="H69" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="I69" s="71" t="s">
+        <v>142</v>
+      </c>
+      <c r="J69" s="71"/>
+      <c r="K69" s="71">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L69" s="71"/>
+    </row>
+    <row r="70" spans="1:12">
       <c r="C70" s="1"/>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="3:5">
+    <row r="71" spans="1:12">
       <c r="C71" s="1"/>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="3:5">
+    <row r="72" spans="1:12">
       <c r="C72" s="1"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="3:5">
+    <row r="73" spans="1:12">
       <c r="C73" s="1"/>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="3:5">
+    <row r="74" spans="1:12">
       <c r="C74" s="1"/>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="3:5">
+    <row r="75" spans="1:12">
       <c r="C75" s="1"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="3:5">
+    <row r="76" spans="1:12">
       <c r="C76" s="1"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="3:5">
+    <row r="77" spans="1:12">
       <c r="C77" s="1"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="3:5">
+    <row r="78" spans="1:12">
       <c r="C78" s="1"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="3:5">
+    <row r="79" spans="1:12">
       <c r="C79" s="1"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="3:5">
+    <row r="80" spans="1:12">
       <c r="C80" s="1"/>
       <c r="E80" s="1"/>
     </row>
@@ -7936,21 +9065,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD990"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="O21" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AC34" sqref="AC34"/>
+      <selection pane="bottomRight" activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="10" width="7" customWidth="1"/>
-    <col min="11" max="30" width="8.1796875" customWidth="1"/>
+    <col min="11" max="30" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="14.5">
+    <row r="1" spans="1:30">
       <c r="A1" s="20" t="s">
         <v>143</v>
       </c>
@@ -7984,7 +9113,7 @@
       <c r="AC1" s="21"/>
       <c r="AD1" s="21"/>
     </row>
-    <row r="2" spans="1:30" ht="14.5">
+    <row r="2" spans="1:30">
       <c r="A2" s="20" t="s">
         <v>144</v>
       </c>
@@ -8018,7 +9147,7 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="21"/>
     </row>
-    <row r="3" spans="1:30" ht="14.5">
+    <row r="3" spans="1:30">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -8050,7 +9179,7 @@
       <c r="AC3" s="21"/>
       <c r="AD3" s="21"/>
     </row>
-    <row r="4" spans="1:30" ht="14.5">
+    <row r="4" spans="1:30">
       <c r="A4" s="22" t="s">
         <v>145</v>
       </c>
@@ -8142,7 +9271,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="14.5">
+    <row r="5" spans="1:30">
       <c r="A5" s="22" t="s">
         <v>25</v>
       </c>
@@ -8241,7 +9370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="14.5">
+    <row r="6" spans="1:30">
       <c r="A6" s="22" t="s">
         <v>32</v>
       </c>
@@ -8341,7 +9470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="14.5">
+    <row r="7" spans="1:30">
       <c r="A7" s="22" t="s">
         <v>36</v>
       </c>
@@ -8438,7 +9567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="14.5">
+    <row r="8" spans="1:30">
       <c r="A8" s="22" t="s">
         <v>41</v>
       </c>
@@ -8536,7 +9665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="14.5">
+    <row r="9" spans="1:30">
       <c r="A9" s="22" t="s">
         <v>46</v>
       </c>
@@ -8635,7 +9764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="14.5">
+    <row r="10" spans="1:30">
       <c r="A10" s="22" t="s">
         <v>51</v>
       </c>
@@ -8735,7 +9864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="14.5">
+    <row r="11" spans="1:30">
       <c r="A11" s="22" t="s">
         <v>56</v>
       </c>
@@ -8838,7 +9967,7 @@
         <v>0.26367831245880025</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="14.5">
+    <row r="12" spans="1:30">
       <c r="A12" s="22" t="s">
         <v>61</v>
       </c>
@@ -8937,7 +10066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="14.5">
+    <row r="13" spans="1:30">
       <c r="A13" s="22" t="s">
         <v>67</v>
       </c>
@@ -9037,7 +10166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="14.5">
+    <row r="14" spans="1:30">
       <c r="A14" s="22" t="s">
         <v>69</v>
       </c>
@@ -41900,11 +43029,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="6" max="6" width="21.26953125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -41926,10 +43055,10 @@
         <v>149</v>
       </c>
       <c r="G2" s="32"/>
-      <c r="H2" s="71" t="s">
+      <c r="H2" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="I2" s="72"/>
+      <c r="I2" s="81"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="33" t="s">

</xml_diff>